<commit_message>
Removed duplicate paper list from P0
</commit_message>
<xml_diff>
--- a/project/P0-pick-papers/PaperChoices2019.xlsx
+++ b/project/P0-pick-papers/PaperChoices2019.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9885" tabRatio="706"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9885" tabRatio="706" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PaperList" sheetId="1" r:id="rId1"/>
@@ -1093,7 +1093,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
@@ -1387,10 +1387,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1453,106 +1453,6 @@
       </c>
       <c r="B7" t="s">
         <v>82</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating paper list and owrking on cm023 solutions.
</commit_message>
<xml_diff>
--- a/project/P0-pick-papers/PaperChoices2019.xlsx
+++ b/project/P0-pick-papers/PaperChoices2019.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="97">
   <si>
     <t>Study</t>
   </si>
@@ -284,6 +284,39 @@
   </si>
   <si>
     <t>David Ross</t>
+  </si>
+  <si>
+    <t>Ally Belikski</t>
+  </si>
+  <si>
+    <t>Dan Fischer</t>
+  </si>
+  <si>
+    <t>Joshua Braunstein</t>
+  </si>
+  <si>
+    <t>Brian Karlberg</t>
+  </si>
+  <si>
+    <t>Raphael Kirchgaessner</t>
+  </si>
+  <si>
+    <t>Meena Mishra</t>
+  </si>
+  <si>
+    <t>Nicole Fontanese</t>
+  </si>
+  <si>
+    <t>Daniel Sobieski</t>
+  </si>
+  <si>
+    <t>Additional Member Required</t>
+  </si>
+  <si>
+    <t>Christina Turner</t>
+  </si>
+  <si>
+    <t>Chris Loo</t>
   </si>
 </sst>
 </file>
@@ -1387,10 +1420,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:A27"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1455,6 +1488,102 @@
         <v>82</v>
       </c>
     </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>4</v>
+      </c>
+      <c r="B13" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>6</v>
+      </c>
+      <c r="B17" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>6</v>
+      </c>
+      <c r="B18" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>6</v>
+      </c>
+      <c r="B19" t="s">
+        <v>94</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:B25">
     <sortCondition ref="A2:A25"/>
@@ -1465,10 +1594,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1562,6 +1691,9 @@
       <c r="B8">
         <v>1</v>
       </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -1570,6 +1702,9 @@
       <c r="B9">
         <v>2</v>
       </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -1578,6 +1713,9 @@
       <c r="B10">
         <v>3</v>
       </c>
+      <c r="C10">
+        <v>8</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -1586,21 +1724,30 @@
       <c r="B11">
         <v>1</v>
       </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B13">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1608,118 +1755,114 @@
         <v>5</v>
       </c>
       <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B15">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
+        <v>6</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
         <v>5</v>
       </c>
-      <c r="B16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>6</v>
       </c>
       <c r="B17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>7</v>
+      </c>
+      <c r="B19">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>6</v>
-      </c>
-      <c r="B19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>7</v>
       </c>
       <c r="B20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>8</v>
+      </c>
+      <c r="B22">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>7</v>
-      </c>
-      <c r="B22">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>8</v>
       </c>
       <c r="B23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>9</v>
+      </c>
+      <c r="B25">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>8</v>
-      </c>
-      <c r="B25">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>9</v>
       </c>
       <c r="B26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>9</v>
-      </c>
-      <c r="B27">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>9</v>
-      </c>
-      <c r="B28">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
cm024 - cm and due. P0 group list.
</commit_message>
<xml_diff>
--- a/project/P0-pick-papers/PaperChoices2019.xlsx
+++ b/project/P0-pick-papers/PaperChoices2019.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9885" tabRatio="706" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9885" tabRatio="706" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="PaperList" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="103">
   <si>
     <t>Study</t>
   </si>
@@ -317,13 +317,31 @@
   </si>
   <si>
     <t>Chris Loo</t>
+  </si>
+  <si>
+    <t>Sonam De</t>
+  </si>
+  <si>
+    <t>Yihua Hu</t>
+  </si>
+  <si>
+    <t>Junhao Qiu</t>
+  </si>
+  <si>
+    <t>Pengxiao Zang</t>
+  </si>
+  <si>
+    <t>Evan Welch</t>
+  </si>
+  <si>
+    <t>Simeneh Woldesenbet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -457,6 +475,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="33">
@@ -800,9 +824,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1420,10 +1447,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1581,6 +1608,54 @@
         <v>6</v>
       </c>
       <c r="B19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>7</v>
+      </c>
+      <c r="B20" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>7</v>
+      </c>
+      <c r="B21" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>7</v>
+      </c>
+      <c r="B22" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>8</v>
+      </c>
+      <c r="B23" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>8</v>
+      </c>
+      <c r="B24" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>8</v>
+      </c>
+      <c r="B25" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1594,10 +1669,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A2" sqref="A2:C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1620,123 +1695,123 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C4">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
         <v>2</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
         <v>2</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6">
-        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
         <v>3</v>
-      </c>
-      <c r="C7">
-        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
         <v>3</v>
       </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
       <c r="C8">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9">
         <v>3</v>
       </c>
-      <c r="B9">
-        <v>2</v>
-      </c>
       <c r="C9">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C10">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12">
         <v>5</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12">
-        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1744,139 +1819,136 @@
         <v>5</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C13">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C15">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C16">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B17">
         <v>3</v>
       </c>
       <c r="C17">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B19">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B20">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B22">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="C22">
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B23">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>9</v>
-      </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>9</v>
-      </c>
-      <c r="B25">
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>9</v>
-      </c>
-      <c r="B26">
-        <v>3</v>
+      <c r="C23">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:C26">
+    <sortCondition ref="C2:C26"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1884,9 +1956,11 @@
     <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>48</v>
       </c>
@@ -1903,111 +1977,99 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="E2" s="1">
-        <v>43440</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <v>2</v>
       </c>
-      <c r="E3" s="1">
-        <v>43440</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D4">
         <v>3</v>
       </c>
-      <c r="E4" s="1">
-        <v>43440</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D5">
         <v>4</v>
       </c>
-      <c r="E5" s="1">
-        <v>43445</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D6">
         <v>5</v>
       </c>
-      <c r="E6" s="1">
-        <v>43445</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C7">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D7">
         <v>6</v>
       </c>
-      <c r="E7" s="1">
-        <v>43445</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -2018,49 +2080,52 @@
       <c r="D8">
         <v>7</v>
       </c>
-      <c r="E8" s="1">
-        <v>43447</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D9">
         <v>8</v>
       </c>
-      <c r="E9" s="1">
-        <v>43447</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>5</v>
-      </c>
-      <c r="D10">
-        <v>9</v>
-      </c>
-      <c r="E10" s="1">
-        <v>43447</v>
-      </c>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E15" s="1"/>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E16" s="1"/>
     </row>
   </sheetData>
-  <sortState ref="A2:E10">
-    <sortCondition ref="D2:D10"/>
+  <sortState ref="A10:C30">
+    <sortCondition ref="A10:A30"/>
+    <sortCondition ref="B10:B30"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Update P0, and post group presentation dates. Working on cm025.Fixed iLab point scale.
</commit_message>
<xml_diff>
--- a/project/P0-pick-papers/PaperChoices2019.xlsx
+++ b/project/P0-pick-papers/PaperChoices2019.xlsx
@@ -19,14 +19,14 @@
     <sheet name="Unused Papers" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Group_Members!$A$1:$B$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Group_Members!$A$1:$B$26</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="104">
   <si>
     <t>Study</t>
   </si>
@@ -310,9 +310,6 @@
     <t>Daniel Sobieski</t>
   </si>
   <si>
-    <t>Additional Member Required</t>
-  </si>
-  <si>
     <t>Christina Turner</t>
   </si>
   <si>
@@ -335,12 +332,21 @@
   </si>
   <si>
     <t>Simeneh Woldesenbet</t>
+  </si>
+  <si>
+    <t>JD Russo</t>
+  </si>
+  <si>
+    <t>PaperName</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm;@"/>
+  </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -826,10 +832,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1154,7 +1160,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1447,10 +1453,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1581,7 +1587,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B16" t="s">
         <v>94</v>
@@ -1605,10 +1611,10 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B19" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1616,7 +1622,7 @@
         <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -1624,15 +1630,15 @@
         <v>7</v>
       </c>
       <c r="B21" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B22" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -1640,7 +1646,7 @@
         <v>8</v>
       </c>
       <c r="B23" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -1648,15 +1654,7 @@
         <v>8</v>
       </c>
       <c r="B24" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>8</v>
-      </c>
-      <c r="B25" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1672,7 +1670,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C23"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1695,123 +1693,123 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
         <v>2</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C7">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C8">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C10">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C11">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B12">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C12">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1819,125 +1817,126 @@
         <v>5</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C14">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C15">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
+        <v>6</v>
+      </c>
+      <c r="B16">
         <v>2</v>
       </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
       <c r="C16">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B17">
         <v>3</v>
       </c>
       <c r="C17">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B18">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C18">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C19">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B20">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C20">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C21">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
+        <v>8</v>
+      </c>
+      <c r="B22">
         <v>2</v>
       </c>
-      <c r="B22">
-        <v>3</v>
-      </c>
       <c r="C22">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B23">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C23">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:C26">
-    <sortCondition ref="C2:C26"/>
+  <sortState ref="A2:C23">
+    <sortCondition ref="A2:A23"/>
+    <sortCondition ref="B2:B23"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1945,10 +1944,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1956,11 +1955,12 @@
     <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>48</v>
       </c>
@@ -1971,13 +1971,16 @@
         <v>51</v>
       </c>
       <c r="D1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" t="s">
         <v>74</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -1987,12 +1990,18 @@
       <c r="C2">
         <v>7</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D2" t="str">
+        <f>VLOOKUP(C2,PaperList!$A$2:$B$14,2)</f>
+        <v>Sleep and eyewitness memory</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2">
+        <v>43804</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2002,12 +2011,18 @@
       <c r="C3">
         <v>2</v>
       </c>
-      <c r="D3">
+      <c r="D3" t="str">
+        <f>VLOOKUP(C3,PaperList!$A$2:$B$14,2)</f>
+        <v>Melodies are social</v>
+      </c>
+      <c r="E3">
         <v>2</v>
       </c>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F3" s="2">
+        <v>43804</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
@@ -2017,12 +2032,18 @@
       <c r="C4">
         <v>3</v>
       </c>
-      <c r="D4">
+      <c r="D4" t="str">
+        <f>VLOOKUP(C4,PaperList!$A$2:$B$14,2)</f>
+        <v>Verbal monitoring in Parkinsons</v>
+      </c>
+      <c r="E4">
         <v>3</v>
       </c>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F4" s="2">
+        <v>43804</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>8</v>
       </c>
@@ -2032,12 +2053,18 @@
       <c r="C5">
         <v>5</v>
       </c>
-      <c r="D5">
+      <c r="D5" t="str">
+        <f>VLOOKUP(C5,PaperList!$A$2:$B$14,2)</f>
+        <v>Visual environment attention</v>
+      </c>
+      <c r="E5">
         <v>4</v>
       </c>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F5" s="2">
+        <v>43809</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
@@ -2047,12 +2074,18 @@
       <c r="C6">
         <v>10</v>
       </c>
-      <c r="D6">
+      <c r="D6" t="str">
+        <f>VLOOKUP(C6,PaperList!$A$2:$B$14,2)</f>
+        <v>Memory for lectures</v>
+      </c>
+      <c r="E6">
         <v>5</v>
       </c>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F6" s="2">
+        <v>43809</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -2062,12 +2095,18 @@
       <c r="C7">
         <v>8</v>
       </c>
-      <c r="D7">
+      <c r="D7" t="str">
+        <f>VLOOKUP(C7,PaperList!$A$2:$B$14,2)</f>
+        <v>Helmets and risk taking</v>
+      </c>
+      <c r="E7">
         <v>6</v>
       </c>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F7" s="2">
+        <v>43809</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2077,12 +2116,18 @@
       <c r="C8">
         <v>1</v>
       </c>
-      <c r="D8">
+      <c r="D8" t="str">
+        <f>VLOOKUP(C8,PaperList!$A$2:$B$14,2)</f>
+        <v>Pain as social glue</v>
+      </c>
+      <c r="E8">
         <v>7</v>
       </c>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F8" s="2">
+        <v>43811</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -2092,32 +2137,19 @@
       <c r="C9">
         <v>6</v>
       </c>
-      <c r="D9">
+      <c r="D9" t="str">
+        <f>VLOOKUP(C9,PaperList!$A$2:$B$14,2)</f>
+        <v>Smartphone addiction</v>
+      </c>
+      <c r="E9">
         <v>8</v>
       </c>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E15" s="1"/>
-      <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E16" s="1"/>
+      <c r="F9" s="2">
+        <v>43811</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H15" s="1"/>
     </row>
   </sheetData>
   <sortState ref="A10:C30">

</xml_diff>